<commit_message>
2 million slopes update
</commit_message>
<xml_diff>
--- a/Tables/bf30_peak_snps.xlsx
+++ b/Tables/bf30_peak_snps.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/AM_Workshop/AM_Workshop/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64DC2F11-20D1-404C-B52F-73C630118CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460D74BF-7539-8B49-B5EC-ED06E24FA46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{0A20FA85-7A3C-AD40-B73A-1B26EC86DA60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Both</t>
   </si>
@@ -56,6 +57,18 @@
   </si>
   <si>
     <t>Bonferonii &amp; select peaks only then filter for BF &gt;10</t>
+  </si>
+  <si>
+    <t>Peak BF &gt; 5 + BF &gt; 30</t>
+  </si>
+  <si>
+    <t>Peak BF &gt; 10 + BF &gt; 20</t>
+  </si>
+  <si>
+    <t>Current MethodPeak BF &gt; 10 + BF &gt; 30</t>
+  </si>
+  <si>
+    <t>Both: Peak BF &gt; 5 + BF &gt; 20</t>
   </si>
 </sst>
 </file>
@@ -427,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A49A937-0063-0F4F-93B8-B2D00DCF2263}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+      <selection activeCell="D3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,8 +506,78 @@
         <v>92</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="C4:D4" si="0">SUM(D2:D3)</f>
+        <f t="shared" ref="D4" si="0">SUM(D2:D3)</f>
         <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4">
+        <v>41</v>
+      </c>
+      <c r="C8" s="4">
+        <v>92</v>
+      </c>
+      <c r="D8" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>330</v>
+      </c>
+      <c r="C9" s="1">
+        <v>664</v>
+      </c>
+      <c r="D9" s="1">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>79</v>
+      </c>
+      <c r="C10" s="1">
+        <v>145</v>
+      </c>
+      <c r="D10" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>368</v>
+      </c>
+      <c r="C11" s="1">
+        <v>717</v>
+      </c>
+      <c r="D11" s="1">
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>